<commit_message>
Hospitality Vending machines 업데이트
#1176
</commit_message>
<xml_diff>
--- a/Data/Adamas/Hospitality Vending machines - 3014885065/3014885065.xlsx
+++ b/Data/Adamas/Hospitality Vending machines - 3014885065/3014885065.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\240122\Hospitality  Vending machines - 3014885065\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Adamas\Hospitality Vending machines - 3014885065\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A0AC3C-FCBA-4E8D-9B72-4A9F3A46EF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F72536F-A4E1-4E97-8E5A-BEFCF9F085A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240128" sheetId="1" r:id="rId1"/>
-    <sheet name="Merge_240128" sheetId="2" r:id="rId2"/>
+    <sheet name="Main_240714" sheetId="3" r:id="rId1"/>
+    <sheet name="Old_240128" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="154">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -432,6 +432,78 @@
   <si>
     <t>중세식 자판기</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> (( RimFridge: Now with Shelves! || RimFridge Updated )) </t>
+  </si>
+  <si>
+    <t>GuestFreeVendingmachine.stages.free_vendingmachine.description</t>
+  </si>
+  <si>
+    <t>ThoughtDef+GuestFreeVendingmachine.stages.free_vendingmachine.description</t>
+  </si>
+  <si>
+    <t>GuestFreeVendingmachine.stages.free_vendingmachine.label</t>
+  </si>
+  <si>
+    <t>ThoughtDef+GuestFreeVendingmachine.stages.free_vendingmachine.label</t>
+  </si>
+  <si>
+    <t>GuestCheapVendingmachine.stages.cheap_vendingmachine.description</t>
+  </si>
+  <si>
+    <t>ThoughtDef+GuestCheapVendingmachine.stages.cheap_vendingmachine.description</t>
+  </si>
+  <si>
+    <t>GuestCheapVendingmachine.stages.cheap_vendingmachine.label</t>
+  </si>
+  <si>
+    <t>ThoughtDef+GuestCheapVendingmachine.stages.cheap_vendingmachine.label</t>
+  </si>
+  <si>
+    <t>GuestExpensiveVendingmachine.stages.expensive_vendingmachine.description</t>
+  </si>
+  <si>
+    <t>ThoughtDef+GuestExpensiveVendingmachine.stages.expensive_vendingmachine.description</t>
+  </si>
+  <si>
+    <t>GuestExpensiveVendingmachine.stages.expensive_vendingmachine.label</t>
+  </si>
+  <si>
+    <t>ThoughtDef+GuestExpensiveVendingmachine.stages.expensive_vendingmachine.label</t>
+  </si>
+  <si>
+    <t>손님이 시설을 이용하도록 허용합니다.</t>
+  </si>
+  <si>
+    <t>누적 수익:</t>
+  </si>
+  <si>
+    <t>현재 수익:</t>
+  </si>
+  <si>
+    <t>TargetA 확인 중</t>
+  </si>
+  <si>
+    <t>자판기 비우는 중</t>
+  </si>
+  <si>
+    <t>손님을 위한 표준적인 자동판매기입니다.</t>
+  </si>
+  <si>
+    <t>중세식 자판기</t>
+  </si>
+  <si>
+    <t>손님을 위한 고전적인 자동판매기입니다. 전기가 필요하지 않습니다.</t>
+  </si>
+  <si>
+    <t>고작 자판기 따위에 많은 돈을 지불해야 했어.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 비우기</t>
+  </si>
+  <si>
+    <t>부패하기 쉬운 음식을 안전하게 판매합니다.</t>
   </si>
 </sst>
 </file>
@@ -782,11 +854,579 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C5BFBE-64D9-4E66-8A03-C40CEB8C4289}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="90.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -795,13 +1435,12 @@
     <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37" style="1" customWidth="1"/>
     <col min="6" max="6" width="45.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +1460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -837,12 +1476,8 @@
       <c r="F2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A2,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>§1을(를) 확인 중입니다.</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -858,12 +1493,8 @@
       <c r="F3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A3,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>자판기를 비우고 있습니다.</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -879,12 +1510,8 @@
       <c r="F4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A4,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>자판기</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -900,12 +1527,8 @@
       <c r="F5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A5,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>투숙객을 위한 표준 자동판매기입니다.</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -921,12 +1544,8 @@
       <c r="F6" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A6,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -942,12 +1561,8 @@
       <c r="F7" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A7,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -963,12 +1578,8 @@
       <c r="F8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A8,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>비싼 자판기</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -984,12 +1595,8 @@
       <c r="F9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A9,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>고작 자판기에 많은 돈을 지불해야 했어.</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1005,12 +1612,8 @@
       <c r="F10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G10" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A10,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>저렴한 자판기</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1026,12 +1629,8 @@
       <c r="F11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A11,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>역시 자판기는 싸야지.</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -1047,12 +1646,8 @@
       <c r="F12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A12,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>무료 자판기</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -1068,12 +1663,8 @@
       <c r="F13" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G13" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A13,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>자판기에 아무것도 지불할 필요가 없었어. 버튼만 누르면 된다고.</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1089,12 +1680,8 @@
       <c r="F14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G14" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A14,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>자판기 비우기</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1110,12 +1697,8 @@
       <c r="F15" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A15,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>자판기 비우기</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -1131,12 +1714,8 @@
       <c r="F16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G16" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A16,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>자판기 비우기</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
@@ -1155,12 +1734,8 @@
       <c r="F17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A17,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>냉장 자판기</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>124</v>
       </c>
@@ -1179,12 +1754,8 @@
       <c r="F18" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G18" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A18,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>부패하기 쉬운 음식을 손님에게 판매하는 자동판매기입니다.</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>125</v>
       </c>
@@ -1203,12 +1774,8 @@
       <c r="F19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A19,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>냉장 자판기</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>126</v>
       </c>
@@ -1227,12 +1794,8 @@
       <c r="F20" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A20,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>부패하기 쉬운 음식을 손님에게 판매하는 자동판매기입니다.</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -1248,12 +1811,8 @@
       <c r="F21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A21,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>자판기</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
@@ -1269,12 +1828,8 @@
       <c r="F22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A22,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>다음을 포함합니다:</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -1290,12 +1845,8 @@
       <c r="F23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A23,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>총 수입:</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -1311,12 +1862,8 @@
       <c r="F24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A24,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>손님이 이 시설을 사용할 수 있도록 허용합니다.</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
@@ -1332,12 +1879,8 @@
       <c r="F25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A25,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>가격 설정</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
@@ -1353,12 +1896,8 @@
       <c r="F26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G26" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A26,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>무료로 제공</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
@@ -1374,12 +1913,8 @@
       <c r="F27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G27" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A27,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>25% 할인 제공</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>84</v>
       </c>
@@ -1395,12 +1930,8 @@
       <c r="F28" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G28" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A28,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>기본 가격</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>87</v>
       </c>
@@ -1416,12 +1947,8 @@
       <c r="F29" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G29" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A29,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>25% 가격 인상</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
@@ -1437,12 +1964,8 @@
       <c r="F30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G30" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A30,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>X시간이 지나면 모든 자판기를 비웁니다.</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>93</v>
       </c>
@@ -1457,370 +1980,10 @@
       </c>
       <c r="F31" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G31" s="1" t="str">
-        <f>IFERROR(VLOOKUP(A31,Merge_240128!$C$2:$D$29,2,FALSE),"")</f>
-        <v>이 시간이 지나도 자동 판매기가 비워지지 않으면 누군가 와서 비워야 합니다.</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D6AE63-12F9-4021-879D-8637D066B626}">
-  <dimension ref="C2:E29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="70" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2">
-        <f>MATCH(C2,Main_240128!$A$2:$A$31,0)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3">
-        <f>MATCH(C3,Main_240128!$A$2:$A$31,0)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4">
-        <f>MATCH(C4,Main_240128!$A$2:$A$31,0)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5">
-        <f>MATCH(C5,Main_240128!$A$2:$A$31,0)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6">
-        <f>MATCH(C6,Main_240128!$A$2:$A$31,0)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7">
-        <f>MATCH(C7,Main_240128!$A$2:$A$31,0)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8">
-        <f>MATCH(C8,Main_240128!$A$2:$A$31,0)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9">
-        <f>MATCH(C9,Main_240128!$A$2:$A$31,0)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10">
-        <f>MATCH(C10,Main_240128!$A$2:$A$31,0)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11">
-        <f>MATCH(C11,Main_240128!$A$2:$A$31,0)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12">
-        <f>MATCH(C12,Main_240128!$A$2:$A$31,0)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13">
-        <f>MATCH(C13,Main_240128!$A$2:$A$31,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14">
-        <f>MATCH(C14,Main_240128!$A$2:$A$31,0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15">
-        <f>MATCH(C15,Main_240128!$A$2:$A$31,0)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16">
-        <f>MATCH(C16,Main_240128!$A$2:$A$31,0)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17">
-        <f>MATCH(C17,Main_240128!$A$2:$A$31,0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18">
-        <f>MATCH(C18,Main_240128!$A$2:$A$31,0)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19">
-        <f>MATCH(C19,Main_240128!$A$2:$A$31,0)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20">
-        <f>MATCH(C20,Main_240128!$A$2:$A$31,0)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21">
-        <f>MATCH(C21,Main_240128!$A$2:$A$31,0)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" t="s">
-        <v>117</v>
-      </c>
-      <c r="E22">
-        <f>MATCH(C22,Main_240128!$A$2:$A$31,0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>118</v>
-      </c>
-      <c r="E23">
-        <f>MATCH(C23,Main_240128!$A$2:$A$31,0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24">
-        <f>MATCH(C24,Main_240128!$A$2:$A$31,0)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E25">
-        <f>MATCH(C25,Main_240128!$A$2:$A$31,0)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26">
-        <f>MATCH(C26,Main_240128!$A$2:$A$31,0)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27">
-        <f>MATCH(C27,Main_240128!$A$2:$A$31,0)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28">
-        <f>MATCH(C28,Main_240128!$A$2:$A$31,0)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29">
-        <f>MATCH(C29,Main_240128!$A$2:$A$31,0)</f>
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>